<commit_message>
presentatie en exel pins
</commit_message>
<xml_diff>
--- a/code/GPIO.xlsx
+++ b/code/GPIO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jarno\Documents\school\20-21\TINPRJ03-34\Git-TINPRJ03-34\code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5061cdd7803951a7/Documenten/Ramon/TI1C/Blok 3/Project 34/Git-TINPRJ03-34/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61CF17D-2FFF-4DF5-A7D0-5EC7C1EE5616}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{A61CF17D-2FFF-4DF5-A7D0-5EC7C1EE5616}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{7034EB76-5D71-4E3C-9D76-0B99E5971D20}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2820" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="19">
   <si>
     <t>K = keypad</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>p</t>
+  </si>
+  <si>
+    <t>Motor 5 euro uit</t>
+  </si>
+  <si>
+    <t>Motor 10 euro uit</t>
+  </si>
+  <si>
+    <t>Motor 20 euro uit</t>
+  </si>
+  <si>
+    <t>Motor 50 euro uit</t>
   </si>
 </sst>
 </file>
@@ -123,7 +135,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -403,13 +415,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -423,7 +438,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -434,7 +449,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -445,7 +460,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -459,7 +474,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -473,7 +488,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -490,7 +505,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -504,7 +519,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -518,7 +533,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -529,7 +544,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -540,7 +555,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -551,7 +566,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -562,7 +577,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -573,7 +588,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -584,7 +599,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
@@ -595,7 +610,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
@@ -609,7 +624,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
@@ -620,7 +635,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
@@ -634,7 +649,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
@@ -648,7 +663,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
@@ -662,7 +677,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
@@ -676,7 +691,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
@@ -690,7 +705,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
@@ -701,7 +716,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>21</v>
       </c>
@@ -715,7 +730,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>22</v>
       </c>
@@ -729,7 +744,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>23</v>
       </c>
@@ -743,7 +758,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>24</v>
       </c>
@@ -754,7 +769,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>25</v>
       </c>
@@ -765,7 +780,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>26</v>
       </c>
@@ -775,8 +790,11 @@
       <c r="C30" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D30" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>27</v>
       </c>
@@ -786,8 +804,11 @@
       <c r="C31" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D31" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>28</v>
       </c>
@@ -797,8 +818,11 @@
       <c r="C32" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>29</v>
       </c>
@@ -808,8 +832,11 @@
       <c r="C33" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>30</v>
       </c>
@@ -819,8 +846,11 @@
       <c r="C34" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D34" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>31</v>
       </c>
@@ -830,8 +860,11 @@
       <c r="C35" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D35" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>32</v>
       </c>
@@ -841,8 +874,11 @@
       <c r="C36" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D36" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>33</v>
       </c>
@@ -852,8 +888,11 @@
       <c r="C37" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D37" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>34</v>
       </c>
@@ -864,7 +903,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>35</v>
       </c>
@@ -875,7 +914,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>36</v>
       </c>
@@ -886,7 +925,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>37</v>
       </c>
@@ -897,7 +936,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>38</v>
       </c>
@@ -908,7 +947,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>39</v>
       </c>

</xml_diff>